<commit_message>
final changes and formatting
</commit_message>
<xml_diff>
--- a/data/semester_average.xlsx
+++ b/data/semester_average.xlsx
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>34.67957746478874</v>
+        <v>35.62025316455696</v>
       </c>
       <c r="C2" t="n">
-        <v>30.52992957746479</v>
+        <v>31.35804701627486</v>
       </c>
       <c r="D2" t="n">
-        <v>33.9031690140845</v>
+        <v>34.82278481012658</v>
       </c>
       <c r="E2" t="n">
-        <v>32.49471830985915</v>
+        <v>33.37613019891501</v>
       </c>
       <c r="F2" t="n">
-        <v>31.0862676056338</v>
+        <v>31.92947558770344</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30.38208409506398</v>
+        <v>31.47537878787879</v>
       </c>
       <c r="C3" t="n">
-        <v>29.80438756855576</v>
+        <v>30.87689393939394</v>
       </c>
       <c r="D3" t="n">
-        <v>30.85374771480804</v>
+        <v>31.96401515151515</v>
       </c>
       <c r="E3" t="n">
-        <v>32.26142595978062</v>
+        <v>33.42234848484848</v>
       </c>
       <c r="F3" t="n">
-        <v>31.74040219378428</v>
+        <v>32.88257575757576</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33.16920473773266</v>
+        <v>34.09217391304348</v>
       </c>
       <c r="C4" t="n">
-        <v>32.20642978003384</v>
+        <v>33.10260869565217</v>
       </c>
       <c r="D4" t="n">
-        <v>33.91032148900169</v>
+        <v>34.85391304347826</v>
       </c>
       <c r="E4" t="n">
-        <v>32.75126903553299</v>
+        <v>33.66260869565217</v>
       </c>
       <c r="F4" t="n">
-        <v>32.99153976311337</v>
+        <v>33.9095652173913</v>
       </c>
     </row>
     <row r="5">
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>35.63405797101449</v>
+        <v>36.35859519408503</v>
       </c>
       <c r="C5" t="n">
-        <v>30.17753623188406</v>
+        <v>30.79112754158965</v>
       </c>
       <c r="D5" t="n">
-        <v>34.39130434782609</v>
+        <v>35.090573012939</v>
       </c>
       <c r="E5" t="n">
-        <v>32.15398550724638</v>
+        <v>32.80776340110906</v>
       </c>
       <c r="F5" t="n">
-        <v>33.90036231884058</v>
+        <v>34.58964879852126</v>
       </c>
     </row>
     <row r="6">
@@ -560,19 +560,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>35.86071428571429</v>
+        <v>37.05166051660517</v>
       </c>
       <c r="C6" t="n">
-        <v>32.70178571428571</v>
+        <v>33.78782287822878</v>
       </c>
       <c r="D6" t="n">
-        <v>30.83214285714286</v>
+        <v>31.85608856088561</v>
       </c>
       <c r="E6" t="n">
-        <v>33.98392857142857</v>
+        <v>35.11254612546126</v>
       </c>
       <c r="F6" t="n">
-        <v>33.22857142857143</v>
+        <v>34.33210332103321</v>
       </c>
     </row>
     <row r="7">
@@ -582,19 +582,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>33.55304347826087</v>
+        <v>34.69964028776978</v>
       </c>
       <c r="C7" t="n">
-        <v>31.29739130434783</v>
+        <v>32.36690647482014</v>
       </c>
       <c r="D7" t="n">
-        <v>34.14260869565217</v>
+        <v>35.30935251798561</v>
       </c>
       <c r="E7" t="n">
-        <v>32.12173913043478</v>
+        <v>33.21942446043165</v>
       </c>
       <c r="F7" t="n">
-        <v>33.34608695652174</v>
+        <v>34.48561151079137</v>
       </c>
     </row>
     <row r="8">
@@ -604,19 +604,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>30.45026178010471</v>
+        <v>31.60869565217391</v>
       </c>
       <c r="C8" t="n">
-        <v>32.66317626527051</v>
+        <v>33.90579710144927</v>
       </c>
       <c r="D8" t="n">
-        <v>32.75741710296684</v>
+        <v>34.0036231884058</v>
       </c>
       <c r="E8" t="n">
-        <v>34.34031413612566</v>
+        <v>35.64673913043478</v>
       </c>
       <c r="F8" t="n">
-        <v>33.28272251308901</v>
+        <v>34.54891304347826</v>
       </c>
     </row>
     <row r="9">
@@ -626,19 +626,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>32.17465753424658</v>
+        <v>33.08098591549296</v>
       </c>
       <c r="C9" t="n">
-        <v>32.38013698630137</v>
+        <v>33.29225352112676</v>
       </c>
       <c r="D9" t="n">
-        <v>30.27739726027397</v>
+        <v>31.13028169014084</v>
       </c>
       <c r="E9" t="n">
-        <v>35.70376712328767</v>
+        <v>36.70950704225352</v>
       </c>
       <c r="F9" t="n">
-        <v>33.09075342465754</v>
+        <v>34.02288732394366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>